<commit_message>
Solo falta una persona para las pruebas y hacer el informe y hablar de sugerencias y errores encontrados con sus soluciones
</commit_message>
<xml_diff>
--- a/tabla METRICAS.xlsx
+++ b/tabla METRICAS.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\UX-Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intercab\AppData\Development\UX-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B4339AE-5C3B-444A-B758-0F36D8A973F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D14A0331-DCF3-4A4B-A5FD-A2D77ECAC890}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>Registrarse</t>
   </si>
@@ -72,12 +71,18 @@
   </si>
   <si>
     <t>Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,9 +163,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -168,6 +170,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,48 +488,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F125B865-9A1D-4216-B4F1-79CA52A2D4F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.77734375" defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="33.88671875" style="1" customWidth="1"/>
-    <col min="4" max="9" width="13.77734375" style="2"/>
+    <col min="3" max="3" width="33.85546875" style="1" customWidth="1"/>
+    <col min="4" max="9" width="13.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -534,12 +543,16 @@
       <c r="E4" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -549,12 +562,16 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
@@ -564,12 +581,16 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
@@ -579,12 +600,16 @@
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
@@ -594,143 +619,175 @@
       <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>3.8194444444444441E-2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>2.5694444444444447E-2</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="5">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.4305555555555556E-2</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>1.5277777777777777E-2</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="5">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1.1805555555555555E-2</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>3.888888888888889E-2</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2.361111111111111E-2</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>3.125E-2</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>3.6805555555555557E-2</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="5">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.2499999999999999E-2</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>2.6388888888888889E-2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="7" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8" t="s">
+      <c r="F17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
@@ -740,12 +797,16 @@
       <c r="E18" s="4">
         <v>9</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="4">
+        <v>14</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
@@ -755,12 +816,16 @@
       <c r="E19" s="4">
         <v>7</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
@@ -770,12 +835,16 @@
       <c r="E20" s="4">
         <v>14</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="4">
+        <v>6</v>
+      </c>
+      <c r="G20" s="4">
+        <v>10</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>2</v>
       </c>
@@ -785,12 +854,16 @@
       <c r="E21" s="4">
         <v>10</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="4">
+        <v>20</v>
+      </c>
+      <c r="G21" s="4">
+        <v>7</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
@@ -800,8 +873,12 @@
       <c r="E22" s="4">
         <v>9</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="4">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>7</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>

</xml_diff>